<commit_message>
U 6 and 0.4 kV
</commit_message>
<xml_diff>
--- a/2.2.xlsx
+++ b/2.2.xlsx
@@ -66,15 +66,9 @@
     <t>ЕКГ-8</t>
   </si>
   <si>
-    <t>Столова</t>
-  </si>
-  <si>
     <t>РРМВ Універсал</t>
   </si>
   <si>
-    <t>АБК ЖДК</t>
-  </si>
-  <si>
     <t>Вибухпром</t>
   </si>
   <si>
@@ -84,12 +78,6 @@
     <t>Промисловий майданчик</t>
   </si>
   <si>
-    <t>Травнсформатор власних потреб</t>
-  </si>
-  <si>
-    <t>Фікальна насосна</t>
-  </si>
-  <si>
     <t>Насоси водовідливу</t>
   </si>
   <si>
@@ -124,6 +112,18 @@
   </si>
   <si>
     <t>S=</t>
+  </si>
+  <si>
+    <t>АБК ЖДЦ</t>
+  </si>
+  <si>
+    <t>Травнсформатор власних потреб (ТМ-40)</t>
+  </si>
+  <si>
+    <t>Їдальня (ТМ-40)</t>
+  </si>
+  <si>
+    <t>Фікальна насосна (ТМ-160)</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -477,13 +480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
@@ -495,50 +498,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -570,8 +573,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
+      <c r="A4" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -603,8 +606,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -635,9 +638,9 @@
         <v>426.49845994019825</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -668,9 +671,9 @@
         <v>737.49576269969168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -702,7 +705,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -735,8 +738,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
+      <c r="A9" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -767,9 +770,9 @@
         <v>1020.2040612204071</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -800,9 +803,9 @@
         <v>1274.9999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -833,9 +836,9 @@
         <v>1431.6094217111663</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>6</v>
@@ -867,6 +870,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="D13" s="1">
         <f>SUM(D3:D12)</f>
         <v>17780</v>
@@ -884,34 +888,38 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
       <c r="G14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="8">
+        <v>22</v>
+      </c>
+      <c r="H14" s="9">
         <f>(H13^2+I13^2)^0.5</f>
         <v>13537.451533751189</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
+      <c r="A16" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -925,8 +933,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
+      <c r="A18" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -939,25 +947,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="D19">
         <f t="shared" si="6"/>
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>SUM(D17:D19)</f>
-        <v>240</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I am going to sleep
</commit_message>
<xml_diff>
--- a/2.2.xlsx
+++ b/2.2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Найменування</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Насоси водовідливу</t>
   </si>
   <si>
-    <t>Бурові верстати СБШ-250</t>
-  </si>
-  <si>
     <t>Бурові верстати СБО-1/20</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Сумарна потужність, кВА</t>
   </si>
   <si>
-    <t>S=</t>
-  </si>
-  <si>
     <t>АБК ЖДЦ</t>
   </si>
   <si>
@@ -124,6 +118,27 @@
   </si>
   <si>
     <t>Фікальна насосна (ТМ-160)</t>
+  </si>
+  <si>
+    <t>Трансформатор власних потреб для екскаваторів ЕКГ-8 (ТМЕ-100)</t>
+  </si>
+  <si>
+    <t>Трансформатор власних потреб для екскаваторів ЕКГ-4 (ТМЕ-40)</t>
+  </si>
+  <si>
+    <t>s=</t>
+  </si>
+  <si>
+    <t>ЕКГ-12</t>
+  </si>
+  <si>
+    <t>Бурові верстати СБШ-320</t>
+  </si>
+  <si>
+    <t>Всього:</t>
+  </si>
+  <si>
+    <t>Трансформатор власних потреб для екскаваторів ЕКГ-12.5 (ТМЕ-250)</t>
   </si>
 </sst>
 </file>
@@ -154,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,41 +177,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,18 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
@@ -497,482 +539,583 @@
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>220</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D12" si="0">C3*B3</f>
-        <v>220</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C3" s="7">
+        <v>630</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3*B3</f>
+        <v>630</v>
+      </c>
+      <c r="E3" s="7">
         <v>0.74</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="7">
         <v>0.6</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="11">
         <f t="shared" ref="G3:G6" si="1">TAN(ACOS(F3))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:H12" si="2">D3*E3</f>
-        <v>162.80000000000001</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H13" si="2">D3*E3</f>
+        <v>466.2</v>
+      </c>
+      <c r="I3" s="7">
         <f>H3*G3</f>
-        <v>217.06666666666666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1">
+        <v>621.59999999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>400</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="7">
         <v>0.7</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="7">
         <v>0.65</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="11">
         <f t="shared" si="1"/>
         <v>1.1691295502746664</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="7">
         <f t="shared" si="2"/>
         <v>280</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" ref="I4:I12" si="3">H4*G4</f>
+      <c r="I4" s="7">
+        <f t="shared" ref="I4:I13" si="3">H4*G4</f>
         <v>327.35627407690657</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <v>320</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="7">
+        <v>630</v>
+      </c>
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-      <c r="E5" s="1">
+        <v>1260</v>
+      </c>
+      <c r="E5" s="7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="7">
         <v>0.65</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="11">
         <f t="shared" si="1"/>
         <v>1.1691295502746664</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="7">
         <f t="shared" si="2"/>
-        <v>364.79999999999995</v>
-      </c>
-      <c r="I5" s="1">
+        <v>718.19999999999993</v>
+      </c>
+      <c r="I5" s="7">
         <f t="shared" si="3"/>
-        <v>426.49845994019825</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+        <v>839.66884300726531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <v>1400</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="7">
+        <v>2500</v>
+      </c>
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-      <c r="E6" s="1">
+        <v>2500</v>
+      </c>
+      <c r="E6" s="7">
         <v>0.85</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="7">
         <v>0.85</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="11">
         <f t="shared" si="1"/>
         <v>0.61974433840310228</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="7">
         <f t="shared" si="2"/>
-        <v>1190</v>
-      </c>
-      <c r="I6" s="1">
+        <v>2125</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" si="3"/>
-        <v>737.49576269969168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+        <v>1316.9567191065923</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>400</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="7">
         <v>0.53</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>0.5</v>
       </c>
-      <c r="G7" s="4">
-        <f t="shared" ref="G7:G12" si="4">TAN(ACOS(F7))</f>
+      <c r="G7" s="11">
+        <f t="shared" ref="G7:G13" si="4">TAN(ACOS(F7))</f>
         <v>1.7320508075688767</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="7">
         <f t="shared" si="2"/>
         <v>424</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="7">
         <f t="shared" si="3"/>
         <v>734.38954240920373</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="7">
         <v>10</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>630</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
         <v>6300</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="7">
         <v>0.45</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="7">
         <v>0.85</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="11">
         <f t="shared" si="4"/>
         <v>0.61974433840310228</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="7">
         <f t="shared" si="2"/>
         <v>2835</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="7">
         <f t="shared" si="3"/>
         <v>1756.975199372795</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>250</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="7">
         <v>0.5</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>0.7</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="11">
         <f t="shared" si="4"/>
         <v>1.0202040612204071</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="7">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="7">
         <f t="shared" si="3"/>
         <v>1020.2040612204071</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
-        <v>250</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="7">
+        <v>1250</v>
+      </c>
+      <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="F10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="7">
         <v>0.8</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="11">
         <f t="shared" si="4"/>
         <v>0.74999999999999978</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="7">
         <f t="shared" si="2"/>
-        <v>1700</v>
-      </c>
-      <c r="I10" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>1274.9999999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
+        <v>3749.9999999999991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>330</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="7">
+        <v>500</v>
+      </c>
+      <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>3300</v>
-      </c>
-      <c r="E11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E11" s="7">
         <v>0.7</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="7">
         <v>0.85</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="11">
         <f t="shared" si="4"/>
         <v>0.61974433840310228</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="7">
         <f t="shared" si="2"/>
-        <v>2310</v>
-      </c>
-      <c r="I11" s="1">
+        <v>3500</v>
+      </c>
+      <c r="I11" s="7">
         <f t="shared" si="3"/>
-        <v>1431.6094217111663</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
+        <v>2169.1051844108579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="7">
         <v>120</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="7">
         <v>0.63</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>0.8</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="11">
         <f t="shared" si="4"/>
         <v>0.74999999999999978</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="7">
         <f t="shared" si="2"/>
         <v>453.6</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="7">
         <f t="shared" si="3"/>
         <v>340.19999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="D13" s="1">
-        <f>SUM(D3:D12)</f>
-        <v>17780</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1">
-        <f t="shared" ref="H13:I13" si="5">SUM(H3:H12)</f>
-        <v>10720.2</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="5"/>
-        <v>8266.7953880970363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="G14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="9">
-        <f>(H13^2+I13^2)^0.5</f>
-        <v>13537.451533751189</v>
-      </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7">
+        <v>400</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="4"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="2"/>
+        <v>2720</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="3"/>
+        <v>2039.9999999999993</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12">
+        <f t="shared" ref="B14:G14" si="5">SUM(D3:D13)</f>
+        <v>32810</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12">
+        <f>SUM(H3:H13)</f>
+        <v>19522</v>
+      </c>
+      <c r="I14" s="12">
+        <f>SUM(I3:I13)</f>
+        <v>14916.455823604028</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="14">
+        <f>(H14^2+I14^2)^0.5</f>
+        <v>24568.458200252015</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="K15">
+        <f>H15+D23</f>
+        <v>28168.458200252015</v>
+      </c>
+      <c r="L15">
+        <f>K15/(2*1.4)</f>
+        <v>10060.163642947149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1">
+        <v>22</v>
+      </c>
+      <c r="B17" s="7">
         <v>2</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>40</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <f>C17*B17</f>
         <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1">
+        <v>23</v>
+      </c>
+      <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="7">
         <v>40</v>
       </c>
-      <c r="D18">
-        <f t="shared" ref="D18:D19" si="6">C18*B18</f>
+      <c r="D18" s="7">
+        <f t="shared" ref="D18:D22" si="6">C18*B18</f>
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="7">
         <v>160</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <f t="shared" si="6"/>
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20">
-        <f>SUM(D17:D19)</f>
-        <v>280</v>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7">
+        <v>10</v>
+      </c>
+      <c r="C20" s="7">
+        <v>100</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>8</v>
+      </c>
+      <c r="C21" s="13">
+        <v>40</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="7">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7">
+        <v>250</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7">
+        <f>SUM(D17:D22)</f>
+        <v>3600</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H14:I14"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -981,6 +1124,6 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I will go to home from university
</commit_message>
<xml_diff>
--- a/2.2.xlsx
+++ b/2.2.xlsx
@@ -219,26 +219,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,40 +540,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="10"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
       <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
       <c r="F3" s="7">
         <v>0.6</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="8">
         <f t="shared" ref="G3:G6" si="1">TAN(ACOS(F3))</f>
         <v>1.3333333333333333</v>
       </c>
@@ -634,7 +634,7 @@
       <c r="F4" s="7">
         <v>0.65</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <f t="shared" si="1"/>
         <v>1.1691295502746664</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="F5" s="7">
         <v>0.65</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <f t="shared" si="1"/>
         <v>1.1691295502746664</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="F6" s="7">
         <v>0.85</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <f t="shared" si="1"/>
         <v>0.61974433840310228</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F7" s="7">
         <v>0.5</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <f t="shared" ref="G7:G13" si="4">TAN(ACOS(F7))</f>
         <v>1.7320508075688767</v>
       </c>
@@ -766,7 +766,7 @@
       <c r="F8" s="7">
         <v>0.85</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <f t="shared" si="4"/>
         <v>0.61974433840310228</v>
       </c>
@@ -799,7 +799,7 @@
       <c r="F9" s="7">
         <v>0.7</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <f t="shared" si="4"/>
         <v>1.0202040612204071</v>
       </c>
@@ -817,14 +817,14 @@
         <v>28</v>
       </c>
       <c r="B10" s="7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10" s="7">
         <v>1250</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>6250</v>
       </c>
       <c r="E10" s="7">
         <v>0.5</v>
@@ -832,17 +832,17 @@
       <c r="F10" s="7">
         <v>0.8</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <f t="shared" si="4"/>
         <v>0.74999999999999978</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>3125</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>3749.9999999999991</v>
+        <v>2343.7499999999991</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
       <c r="F11" s="7">
         <v>0.85</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <f t="shared" si="4"/>
         <v>0.61974433840310228</v>
       </c>
@@ -898,7 +898,7 @@
       <c r="F12" s="7">
         <v>0.8</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <f t="shared" si="4"/>
         <v>0.74999999999999978</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="F13" s="7">
         <v>0.8</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <f t="shared" si="4"/>
         <v>0.74999999999999978</v>
       </c>
@@ -949,7 +949,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="11"/>
+      <c r="S13" s="8"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
@@ -957,22 +957,22 @@
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12">
-        <f t="shared" ref="B14:G14" si="5">SUM(D3:D13)</f>
-        <v>32810</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9">
+        <f t="shared" ref="D14" si="5">SUM(D3:D13)</f>
+        <v>29060</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <f>SUM(H3:H13)</f>
-        <v>19522</v>
-      </c>
-      <c r="I14" s="12">
+        <v>17647</v>
+      </c>
+      <c r="I14" s="9">
         <f>SUM(I3:I13)</f>
-        <v>14916.455823604028</v>
+        <v>13510.205823604028</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -980,18 +980,18 @@
       <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="11">
         <f>(H14^2+I14^2)^0.5</f>
-        <v>24568.458200252015</v>
-      </c>
-      <c r="I15" s="14"/>
+        <v>22224.812044112863</v>
+      </c>
+      <c r="I15" s="11"/>
       <c r="K15">
         <f>H15+D23</f>
-        <v>28168.458200252015</v>
+        <v>25074.812044112863</v>
       </c>
       <c r="L15">
         <f>K15/(2*1.4)</f>
-        <v>10060.163642947149</v>
+        <v>8955.2900157545937</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1070,14 +1070,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="10">
         <v>8</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="10">
         <v>40</v>
       </c>
       <c r="D21" s="7">
@@ -1085,22 +1085,23 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="7">
-        <v>8</v>
+        <f>B10</f>
+        <v>5</v>
       </c>
       <c r="C22" s="7">
         <v>250</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
@@ -1108,7 +1109,17 @@
       <c r="C23" s="4"/>
       <c r="D23" s="7">
         <f>SUM(D17:D22)</f>
-        <v>3600</v>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>D23+H15</f>
+        <v>25074.812044112863</v>
+      </c>
+      <c r="H24">
+        <f>G24/(2*0.8)</f>
+        <v>15671.757527570539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I go to sleep
</commit_message>
<xml_diff>
--- a/2.2.xlsx
+++ b/2.2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Найменування</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Трансформатор власних потреб для екскаваторів ЕКГ-12.5 (ТМЕ-250)</t>
+  </si>
+  <si>
+    <t>Kз</t>
+  </si>
+  <si>
+    <t>Kз.ав</t>
+  </si>
+  <si>
+    <t>I35</t>
+  </si>
+  <si>
+    <t>I6</t>
   </si>
 </sst>
 </file>
@@ -522,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,8 +1021,15 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16">
+        <f>K15/(3^(1/2)*35)</f>
+        <v>413.62712810136662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1024,8 +1043,15 @@
         <f>C17*B17</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17">
+        <f>K15/(3^(1/2)*6)</f>
+        <v>2412.8249139246386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1040,7 +1066,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1081,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1096,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1111,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1101,7 +1127,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
@@ -1112,7 +1138,7 @@
         <v>2850</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G24">
         <f>D23+H15</f>
         <v>25074.812044112863</v>
@@ -1122,13 +1148,19 @@
         <v>15985.19267812195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
       <c r="G26">
         <f>(H24*1.02)/(2*16000)</f>
         <v>0.50952801661513714</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
       <c r="G27">
         <f>(H24*1.02)/(1*16000)</f>
         <v>1.0190560332302743</v>

</xml_diff>